<commit_message>
updating test data sheet with new user
</commit_message>
<xml_diff>
--- a/TestData/AppData.xlsx
+++ b/TestData/AppData.xlsx
@@ -18,20 +18,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>ballu@gmail.com</t>
+    <t>tallu@gmail.com</t>
   </si>
   <si>
-    <t>ballu</t>
+    <t>tallu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,13 +62,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,7 +374,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +384,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -381,6 +392,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>